<commit_message>
working sample of the a google action publishing information file generation
</commit_message>
<xml_diff>
--- a/test/spreadsheets/Voxa Cli Intents Utterances en-US.xlsx
+++ b/test/spreadsheets/Voxa Cli Intents Utterances en-US.xlsx
@@ -1088,14 +1088,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.19"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,7 +1332,7 @@
         <v>54</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>55</v>
@@ -1355,7 +1355,7 @@
     <hyperlink ref="B13" r:id="rId2" display="https://example.com/terms"/>
     <hyperlink ref="B20" r:id="rId3" display="developer@example.com"/>
     <hyperlink ref="B21" r:id="rId4" display="https://example.com/terms"/>
-    <hyperlink ref="B24" r:id="rId5" display="https://example.com/terms"/>
+    <hyperlink ref="B24" r:id="rId5" display="https://example.com/policy"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1380,7 +1380,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.05"/>
@@ -1452,7 +1452,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="42.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="47.62"/>
@@ -1543,7 +1543,7 @@
       <selection pane="bottomLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="74.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.16"/>
@@ -1893,7 +1893,7 @@
       <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.39453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.58"/>
@@ -2190,7 +2190,7 @@
       <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.39453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.28"/>
@@ -2306,7 +2306,7 @@
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.83"/>
   </cols>
@@ -2355,7 +2355,7 @@
       <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.64453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="87.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.27"/>
@@ -2409,9 +2409,9 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.39453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.36"/>
   </cols>
   <sheetData>
@@ -2449,7 +2449,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.39453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.36"/>
@@ -2503,7 +2503,7 @@
       <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.39453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.36"/>

</xml_diff>